<commit_message>
Updated README.md && Test Run #2
</commit_message>
<xml_diff>
--- a/asl_abstract_dataset/labels.xlsx
+++ b/asl_abstract_dataset/labels.xlsx
@@ -450,7 +450,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.990886569342717</v>
+        <v>4.695084332872982</v>
       </c>
     </row>
     <row r="3">
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3.318898527172568</v>
+        <v>1.367822428585241</v>
       </c>
     </row>
     <row r="4">
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4.504899046671653</v>
+        <v>1.373416562516416</v>
       </c>
     </row>
     <row r="5">
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.641710959498223</v>
+        <v>2.793182710808981</v>
       </c>
     </row>
     <row r="6">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2.927448143361745</v>
+        <v>3.20821025510794</v>
       </c>
     </row>
     <row r="7">
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2.811822079814595</v>
+        <v>1.659877161529454</v>
       </c>
     </row>
     <row r="8">
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2.683938247643774</v>
+        <v>2.489421575316852</v>
       </c>
     </row>
     <row r="9">
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.052280297489216</v>
+        <v>1.076942157917816</v>
       </c>
     </row>
     <row r="10">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.973025918541857</v>
+        <v>1.742102883324863</v>
       </c>
     </row>
     <row r="11">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1.572837609592973</v>
+        <v>1.051539574900377</v>
       </c>
     </row>
     <row r="12">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3.018128261291763</v>
+        <v>1.471378068340352</v>
       </c>
     </row>
     <row r="13">
@@ -615,7 +615,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1.590219512707643</v>
+        <v>2.45598214833424</v>
       </c>
     </row>
     <row r="14">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3.192875021503046</v>
+        <v>2.168829216199613</v>
       </c>
     </row>
     <row r="15">
@@ -645,7 +645,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3.794461361634037</v>
+        <v>1.319197212752667</v>
       </c>
     </row>
     <row r="16">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3.707739253217991</v>
+        <v>2.701765945510142</v>
       </c>
     </row>
     <row r="17">
@@ -675,7 +675,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4.416229930998187</v>
+        <v>3.959827860569702</v>
       </c>
     </row>
     <row r="18">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1.943081028850839</v>
+        <v>4.780815649798236</v>
       </c>
     </row>
     <row r="19">
@@ -705,7 +705,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2.651221773013836</v>
+        <v>1.483375813531296</v>
       </c>
     </row>
     <row r="20">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>4.268515399005203</v>
+        <v>3.259976367187397</v>
       </c>
     </row>
     <row r="21">
@@ -735,7 +735,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>4.785678636217181</v>
+        <v>2.084543233313333</v>
       </c>
     </row>
     <row r="22">
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>4.313326179756505</v>
+        <v>3.517028096133118</v>
       </c>
     </row>
     <row r="23">
@@ -765,7 +765,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2.902857528664092</v>
+        <v>3.085210297917973</v>
       </c>
     </row>
     <row r="24">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1.813494947175751</v>
+        <v>2.356770184592987</v>
       </c>
     </row>
     <row r="25">
@@ -795,7 +795,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2.828920824388625</v>
+        <v>4.511659143276358</v>
       </c>
     </row>
     <row r="26">
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3.615498762980764</v>
+        <v>1.155851012556151</v>
       </c>
     </row>
     <row r="27">
@@ -825,7 +825,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>3.791340654654104</v>
+        <v>4.834766207493523</v>
       </c>
     </row>
     <row r="28">
@@ -840,7 +840,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2.463158284269457</v>
+        <v>4.553185433283713</v>
       </c>
     </row>
     <row r="29">
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1.316787248086564</v>
+        <v>2.437784576169393</v>
       </c>
     </row>
     <row r="30">
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>3.626861191257017</v>
+        <v>3.863222124052614</v>
       </c>
     </row>
     <row r="31">
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1.609855225362856</v>
+        <v>2.88544459640559</v>
       </c>
     </row>
     <row r="32">
@@ -900,7 +900,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>4.64225702432597</v>
+        <v>4.163054992766253</v>
       </c>
     </row>
     <row r="33">
@@ -915,7 +915,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>4.811726028039221</v>
+        <v>3.121448339320306</v>
       </c>
     </row>
     <row r="34">
@@ -930,7 +930,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>4.789971526136625</v>
+        <v>3.151787253776842</v>
       </c>
     </row>
     <row r="35">
@@ -945,7 +945,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2.516170933507699</v>
+        <v>1.463538871984101</v>
       </c>
     </row>
     <row r="36">
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>4.052965543863669</v>
+        <v>4.635420578698104</v>
       </c>
     </row>
     <row r="37">
@@ -975,7 +975,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1.181469989482399</v>
+        <v>1.988686998907551</v>
       </c>
     </row>
     <row r="38">
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2.431636521673251</v>
+        <v>2.518737126700775</v>
       </c>
     </row>
     <row r="39">
@@ -1005,7 +1005,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1.111275085143061</v>
+        <v>2.108507899108561</v>
       </c>
     </row>
     <row r="40">
@@ -1020,7 +1020,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>4.836328049370481</v>
+        <v>2.240516371872697</v>
       </c>
     </row>
     <row r="41">
@@ -1035,7 +1035,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.120140901413175</v>
+        <v>2.910354227965352</v>
       </c>
     </row>
     <row r="42">
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>3.10799374721388</v>
+        <v>4.393465305599065</v>
       </c>
     </row>
     <row r="43">
@@ -1065,7 +1065,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>3.356139224797805</v>
+        <v>3.10771430294957</v>
       </c>
     </row>
     <row r="44">
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1.145405977948572</v>
+        <v>3.373152493001212</v>
       </c>
     </row>
     <row r="45">
@@ -1095,7 +1095,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>4.959718364612826</v>
+        <v>3.383037315981646</v>
       </c>
     </row>
     <row r="46">
@@ -1110,7 +1110,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1.434570225700445</v>
+        <v>2.454312766833199</v>
       </c>
     </row>
     <row r="47">
@@ -1125,7 +1125,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1.011448472196276</v>
+        <v>3.858424891152243</v>
       </c>
     </row>
     <row r="48">
@@ -1140,7 +1140,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>2.671978103475379</v>
+        <v>4.955612235924578</v>
       </c>
     </row>
     <row r="49">
@@ -1155,7 +1155,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.164549668175094</v>
+        <v>4.399447889783206</v>
       </c>
     </row>
     <row r="50">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>2.737671075392803</v>
+        <v>1.620075997407123</v>
       </c>
     </row>
     <row r="51">
@@ -1185,7 +1185,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4.435020542182216</v>
+        <v>4.155583451474263</v>
       </c>
     </row>
     <row r="52">
@@ -1200,7 +1200,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>3.599612847192468</v>
+        <v>1.974929065659646</v>
       </c>
     </row>
     <row r="53">
@@ -1215,7 +1215,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1.038157888918399</v>
+        <v>2.649445895641659</v>
       </c>
     </row>
     <row r="54">
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3.955652963092289</v>
+        <v>1.263214280790705</v>
       </c>
     </row>
     <row r="55">
@@ -1245,7 +1245,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1.322281036295892</v>
+        <v>2.246260911247175</v>
       </c>
     </row>
     <row r="56">
@@ -1260,7 +1260,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2.700541768953979</v>
+        <v>4.798010892389836</v>
       </c>
     </row>
     <row r="57">
@@ -1275,7 +1275,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>3.661340399990964</v>
+        <v>1.706977204339176</v>
       </c>
     </row>
     <row r="58">
@@ -1290,7 +1290,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>2.955341265816533</v>
+        <v>3.715058342088656</v>
       </c>
     </row>
     <row r="59">
@@ -1305,7 +1305,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2.910705189141892</v>
+        <v>4.912829523758626</v>
       </c>
     </row>
     <row r="60">
@@ -1320,7 +1320,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1.175743584690542</v>
+        <v>1.478964082425837</v>
       </c>
     </row>
     <row r="61">
@@ -1335,7 +1335,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2.815215149387895</v>
+        <v>2.640047011060466</v>
       </c>
     </row>
     <row r="62">
@@ -1350,7 +1350,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1.856365364481232</v>
+        <v>2.692234938221178</v>
       </c>
     </row>
     <row r="63">
@@ -1365,7 +1365,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>3.128981114876883</v>
+        <v>4.247810721877821</v>
       </c>
     </row>
     <row r="64">
@@ -1380,7 +1380,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2.466733816685645</v>
+        <v>4.752151299888917</v>
       </c>
     </row>
     <row r="65">
@@ -1395,7 +1395,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>3.278143847201138</v>
+        <v>3.199600370680892</v>
       </c>
     </row>
     <row r="66">
@@ -1410,7 +1410,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2.790310082275215</v>
+        <v>3.673293652862804</v>
       </c>
     </row>
     <row r="67">
@@ -1425,7 +1425,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1.8413834482158</v>
+        <v>1.40484476466401</v>
       </c>
     </row>
     <row r="68">
@@ -1440,7 +1440,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>4.916926757559187</v>
+        <v>2.399781930768144</v>
       </c>
     </row>
     <row r="69">
@@ -1455,7 +1455,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>3.364137410963006</v>
+        <v>4.879897454819279</v>
       </c>
     </row>
     <row r="70">
@@ -1470,7 +1470,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>2.203194903368331</v>
+        <v>1.200887677681637</v>
       </c>
     </row>
     <row r="71">
@@ -1485,7 +1485,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>2.769382222616333</v>
+        <v>1.853030211501316</v>
       </c>
     </row>
     <row r="72">
@@ -1500,7 +1500,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>4.109719375201379</v>
+        <v>2.271167986000254</v>
       </c>
     </row>
     <row r="73">
@@ -1515,7 +1515,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>3.599576517238285</v>
+        <v>2.415151096492064</v>
       </c>
     </row>
     <row r="74">
@@ -1530,7 +1530,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>3.399268236520462</v>
+        <v>4.374804070115606</v>
       </c>
     </row>
     <row r="75">
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1.048764309365054</v>
+        <v>1.54164045546619</v>
       </c>
     </row>
     <row r="76">
@@ -1560,7 +1560,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>2.992556419621756</v>
+        <v>1.299419193086417</v>
       </c>
     </row>
     <row r="77">
@@ -1575,7 +1575,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>4.304375496522852</v>
+        <v>4.148579090879959</v>
       </c>
     </row>
     <row r="78">
@@ -1590,7 +1590,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>1.259486453300421</v>
+        <v>4.642826251974615</v>
       </c>
     </row>
     <row r="79">
@@ -1605,7 +1605,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>4.129905789936677</v>
+        <v>3.694348296018784</v>
       </c>
     </row>
     <row r="80">
@@ -1620,7 +1620,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1.294717068800872</v>
+        <v>2.84890418230593</v>
       </c>
     </row>
     <row r="81">
@@ -1635,7 +1635,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>1.935244679667748</v>
+        <v>3.363686770856152</v>
       </c>
     </row>
     <row r="82">
@@ -1650,7 +1650,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>3.493853514568806</v>
+        <v>1.408079058869165</v>
       </c>
     </row>
     <row r="83">
@@ -1665,7 +1665,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>4.041554405063509</v>
+        <v>1.588389506577446</v>
       </c>
     </row>
     <row r="84">
@@ -1680,7 +1680,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>3.674874979244342</v>
+        <v>2.913386135446874</v>
       </c>
     </row>
     <row r="85">
@@ -1695,7 +1695,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>1.540133371310837</v>
+        <v>4.529774062777629</v>
       </c>
     </row>
     <row r="86">
@@ -1710,7 +1710,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>2.701476233516094</v>
+        <v>1.308616110587125</v>
       </c>
     </row>
     <row r="87">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>4.593185089195099</v>
+        <v>1.765601495249265</v>
       </c>
     </row>
     <row r="88">
@@ -1740,7 +1740,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>1.093611804142448</v>
+        <v>1.780984670932191</v>
       </c>
     </row>
     <row r="89">
@@ -1755,7 +1755,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>3.044460607556644</v>
+        <v>1.993718273529824</v>
       </c>
     </row>
     <row r="90">
@@ -1770,7 +1770,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>1.174477429539036</v>
+        <v>2.185714309524625</v>
       </c>
     </row>
     <row r="91">
@@ -1785,7 +1785,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>4.143432397223199</v>
+        <v>3.942020725821648</v>
       </c>
     </row>
     <row r="92">
@@ -1800,7 +1800,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>2.843177644036372</v>
+        <v>4.756795033168359</v>
       </c>
     </row>
     <row r="93">
@@ -1815,7 +1815,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>3.197815359282613</v>
+        <v>3.93164833869365</v>
       </c>
     </row>
     <row r="94">
@@ -1830,7 +1830,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>2.145587694804703</v>
+        <v>2.379160427075865</v>
       </c>
     </row>
     <row r="95">
@@ -1845,7 +1845,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>3.628117952646184</v>
+        <v>4.077991734886929</v>
       </c>
     </row>
     <row r="96">
@@ -1860,7 +1860,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1.917479319010453</v>
+        <v>4.045817961571915</v>
       </c>
     </row>
     <row r="97">
@@ -1875,7 +1875,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>4.842713656897038</v>
+        <v>1.460808969459078</v>
       </c>
     </row>
     <row r="98">
@@ -1890,7 +1890,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>3.601260983684869</v>
+        <v>3.565297422907259</v>
       </c>
     </row>
     <row r="99">
@@ -1905,7 +1905,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>3.318122276075154</v>
+        <v>4.509719408079015</v>
       </c>
     </row>
     <row r="100">
@@ -1920,7 +1920,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>4.681821601863829</v>
+        <v>2.155476625523117</v>
       </c>
     </row>
     <row r="101">
@@ -1935,7 +1935,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>1.88128648323226</v>
+        <v>4.219400700171475</v>
       </c>
     </row>
     <row r="102">
@@ -1950,7 +1950,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>3.206331166608773</v>
+        <v>3.835730955381725</v>
       </c>
     </row>
     <row r="103">
@@ -1965,7 +1965,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1.54871387612207</v>
+        <v>4.597066185223494</v>
       </c>
     </row>
     <row r="104">
@@ -1980,7 +1980,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>4.83660480627965</v>
+        <v>4.890951756406528</v>
       </c>
     </row>
     <row r="105">
@@ -1995,7 +1995,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>4.725024568868742</v>
+        <v>1.656735071500933</v>
       </c>
     </row>
     <row r="106">
@@ -2010,7 +2010,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1.137205612690712</v>
+        <v>4.096316417824946</v>
       </c>
     </row>
     <row r="107">
@@ -2025,7 +2025,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>3.139408011267022</v>
+        <v>3.92317108166597</v>
       </c>
     </row>
     <row r="108">
@@ -2040,7 +2040,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>1.847859059968166</v>
+        <v>4.791975903074427</v>
       </c>
     </row>
     <row r="109">
@@ -2055,7 +2055,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>1.906204770560769</v>
+        <v>2.846599226165412</v>
       </c>
     </row>
     <row r="110">
@@ -2070,7 +2070,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>4.84632277371959</v>
+        <v>3.057673468867839</v>
       </c>
     </row>
     <row r="111">
@@ -2085,7 +2085,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>2.225640826284286</v>
+        <v>2.892736083865604</v>
       </c>
     </row>
     <row r="112">
@@ -2100,7 +2100,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>4.345546870609107</v>
+        <v>3.870965965567564</v>
       </c>
     </row>
     <row r="113">
@@ -2115,7 +2115,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>3.228497236685969</v>
+        <v>1.799624558936146</v>
       </c>
     </row>
     <row r="114">
@@ -2130,7 +2130,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>3.053733114267074</v>
+        <v>1.048731638354134</v>
       </c>
     </row>
     <row r="115">
@@ -2145,7 +2145,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>1.480319735409518</v>
+        <v>4.633357331617381</v>
       </c>
     </row>
     <row r="116">
@@ -2160,7 +2160,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>2.747360004945769</v>
+        <v>4.122014071441197</v>
       </c>
     </row>
     <row r="117">
@@ -2175,7 +2175,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>4.250866317560956</v>
+        <v>2.408622318713953</v>
       </c>
     </row>
     <row r="118">
@@ -2190,7 +2190,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>2.697103455006898</v>
+        <v>2.014756113633208</v>
       </c>
     </row>
     <row r="119">
@@ -2205,7 +2205,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>4.609813893827013</v>
+        <v>4.337969252047911</v>
       </c>
     </row>
     <row r="120">
@@ -2220,7 +2220,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>3.801068523252248</v>
+        <v>4.179661511945971</v>
       </c>
     </row>
     <row r="121">
@@ -2235,7 +2235,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>3.451166042797051</v>
+        <v>2.600418746562025</v>
       </c>
     </row>
     <row r="122">
@@ -2250,7 +2250,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2.033890898674703</v>
+        <v>4.140814401211582</v>
       </c>
     </row>
     <row r="123">
@@ -2265,7 +2265,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>3.871721408354451</v>
+        <v>2.740667278886615</v>
       </c>
     </row>
     <row r="124">
@@ -2280,7 +2280,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1.268891725666181</v>
+        <v>2.209665051119308</v>
       </c>
     </row>
     <row r="125">
@@ -2295,7 +2295,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>3.751065918558567</v>
+        <v>3.317374393384631</v>
       </c>
     </row>
     <row r="126">
@@ -2310,7 +2310,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>3.844927946317548</v>
+        <v>1.849116489603116</v>
       </c>
     </row>
     <row r="127">
@@ -2325,7 +2325,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>4.490179027538719</v>
+        <v>3.242319087675397</v>
       </c>
     </row>
     <row r="128">
@@ -2340,7 +2340,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>3.113144030706027</v>
+        <v>2.160278063848186</v>
       </c>
     </row>
     <row r="129">
@@ -2355,7 +2355,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>3.803767679218983</v>
+        <v>4.268911765692625</v>
       </c>
     </row>
     <row r="130">
@@ -2370,7 +2370,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>3.246118098558507</v>
+        <v>1.199680387014284</v>
       </c>
     </row>
     <row r="131">
@@ -2385,7 +2385,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1.795652373539248</v>
+        <v>3.564458894657954</v>
       </c>
     </row>
     <row r="132">
@@ -2400,7 +2400,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>4.591254238159884</v>
+        <v>1.556040778517771</v>
       </c>
     </row>
     <row r="133">
@@ -2415,7 +2415,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>1.588623290419938</v>
+        <v>3.024658324580154</v>
       </c>
     </row>
     <row r="134">
@@ -2430,7 +2430,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>3.533424947736617</v>
+        <v>1.388538630857336</v>
       </c>
     </row>
     <row r="135">
@@ -2445,7 +2445,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>3.091139209447242</v>
+        <v>3.171420434603725</v>
       </c>
     </row>
     <row r="136">
@@ -2460,7 +2460,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>1.479163284778259</v>
+        <v>3.520374922189444</v>
       </c>
     </row>
     <row r="137">
@@ -2475,7 +2475,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>1.301472259205368</v>
+        <v>2.99460170481184</v>
       </c>
     </row>
     <row r="138">
@@ -2490,7 +2490,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>1.877698136194255</v>
+        <v>4.727059134401256</v>
       </c>
     </row>
     <row r="139">
@@ -2505,7 +2505,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>2.261890046898342</v>
+        <v>3.848678983497988</v>
       </c>
     </row>
     <row r="140">
@@ -2520,7 +2520,7 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>3.390214662941516</v>
+        <v>1.293998032380085</v>
       </c>
     </row>
     <row r="141">
@@ -2535,7 +2535,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>3.736139223847609</v>
+        <v>1.639762429134358</v>
       </c>
     </row>
     <row r="142">
@@ -2550,7 +2550,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>4.672003593144612</v>
+        <v>4.425667127632858</v>
       </c>
     </row>
     <row r="143">
@@ -2565,7 +2565,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>2.831674326277849</v>
+        <v>3.54830962231801</v>
       </c>
     </row>
     <row r="144">
@@ -2580,7 +2580,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>1.799423237373568</v>
+        <v>1.112730614946265</v>
       </c>
     </row>
     <row r="145">
@@ -2595,7 +2595,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>4.252563507080572</v>
+        <v>1.424750429833481</v>
       </c>
     </row>
     <row r="146">
@@ -2610,7 +2610,7 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>4.706960385385031</v>
+        <v>3.12316633972422</v>
       </c>
     </row>
     <row r="147">
@@ -2625,7 +2625,7 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>4.313050601210302</v>
+        <v>2.811859835037253</v>
       </c>
     </row>
     <row r="148">
@@ -2640,7 +2640,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>2.724097731357543</v>
+        <v>3.100002380883957</v>
       </c>
     </row>
     <row r="149">
@@ -2655,7 +2655,7 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>4.458336179385727</v>
+        <v>4.633876401767178</v>
       </c>
     </row>
     <row r="150">
@@ -2670,7 +2670,7 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>2.675715841387557</v>
+        <v>2.907605477380031</v>
       </c>
     </row>
     <row r="151">
@@ -2685,7 +2685,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>3.175912384548143</v>
+        <v>4.113899491722985</v>
       </c>
     </row>
     <row r="152">
@@ -2700,7 +2700,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>2.592540315227355</v>
+        <v>1.05170852817511</v>
       </c>
     </row>
     <row r="153">
@@ -2715,7 +2715,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>3.72029174452049</v>
+        <v>2.315556527253207</v>
       </c>
     </row>
     <row r="154">
@@ -2730,7 +2730,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>2.242883948866867</v>
+        <v>2.469869396164805</v>
       </c>
     </row>
     <row r="155">
@@ -2745,7 +2745,7 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>3.218296239232172</v>
+        <v>1.863193139234976</v>
       </c>
     </row>
     <row r="156">
@@ -2760,7 +2760,7 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>2.90446548114206</v>
+        <v>1.113028509114417</v>
       </c>
     </row>
     <row r="157">
@@ -2775,7 +2775,7 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>3.084797253940073</v>
+        <v>1.800705688982124</v>
       </c>
     </row>
     <row r="158">
@@ -2790,7 +2790,7 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>2.017342346561176</v>
+        <v>2.197453124060817</v>
       </c>
     </row>
     <row r="159">
@@ -2805,7 +2805,7 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>1.914830108291828</v>
+        <v>3.497309213606365</v>
       </c>
     </row>
     <row r="160">
@@ -2820,7 +2820,7 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>4.812243160107345</v>
+        <v>4.801932113409026</v>
       </c>
     </row>
     <row r="161">
@@ -2835,7 +2835,7 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>4.184354861839379</v>
+        <v>1.054691720778581</v>
       </c>
     </row>
     <row r="162">
@@ -2850,7 +2850,7 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>2.753992402272657</v>
+        <v>3.879059222006379</v>
       </c>
     </row>
     <row r="163">
@@ -2865,7 +2865,7 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>2.857196902487202</v>
+        <v>3.793299400872682</v>
       </c>
     </row>
     <row r="164">
@@ -2880,7 +2880,7 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>3.666566653179469</v>
+        <v>4.297181206858704</v>
       </c>
     </row>
     <row r="165">
@@ -2895,7 +2895,7 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>3.446728245979901</v>
+        <v>2.648922567544651</v>
       </c>
     </row>
     <row r="166">
@@ -2910,7 +2910,7 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>3.079377430926297</v>
+        <v>3.111072112358583</v>
       </c>
     </row>
     <row r="167">
@@ -2925,7 +2925,7 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>3.242684408258137</v>
+        <v>4.70128779194197</v>
       </c>
     </row>
     <row r="168">
@@ -2940,7 +2940,7 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>2.003015940543525</v>
+        <v>4.705247003453916</v>
       </c>
     </row>
     <row r="169">
@@ -2955,7 +2955,7 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>2.958188814371583</v>
+        <v>2.183886550316979</v>
       </c>
     </row>
     <row r="170">
@@ -2970,7 +2970,7 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>2.430545606911438</v>
+        <v>4.591738596710542</v>
       </c>
     </row>
     <row r="171">
@@ -2985,7 +2985,7 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>3.3831813272972</v>
+        <v>3.316293877503367</v>
       </c>
     </row>
     <row r="172">
@@ -3000,7 +3000,7 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>1.700796410664231</v>
+        <v>3.476616869004758</v>
       </c>
     </row>
     <row r="173">
@@ -3015,7 +3015,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>4.185491569394463</v>
+        <v>1.028722067137714</v>
       </c>
     </row>
     <row r="174">
@@ -3030,7 +3030,7 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>2.122170775789049</v>
+        <v>2.713672233748871</v>
       </c>
     </row>
     <row r="175">
@@ -3045,7 +3045,7 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>3.105668565117606</v>
+        <v>2.573118245164172</v>
       </c>
     </row>
     <row r="176">
@@ -3060,7 +3060,7 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>2.180922123513211</v>
+        <v>3.453953840603064</v>
       </c>
     </row>
     <row r="177">
@@ -3075,7 +3075,7 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>1.688194675895105</v>
+        <v>3.649915255940351</v>
       </c>
     </row>
     <row r="178">
@@ -3090,7 +3090,7 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>3.239395628624729</v>
+        <v>4.632452490250246</v>
       </c>
     </row>
     <row r="179">
@@ -3105,7 +3105,7 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>2.47084761518394</v>
+        <v>1.34254864100054</v>
       </c>
     </row>
     <row r="180">
@@ -3120,7 +3120,7 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>1.321873549709929</v>
+        <v>1.256140641327201</v>
       </c>
     </row>
     <row r="181">
@@ -3135,7 +3135,7 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>4.326843840272014</v>
+        <v>1.305782086585742</v>
       </c>
     </row>
     <row r="182">
@@ -3150,7 +3150,7 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>3.461160511936055</v>
+        <v>4.563613803027619</v>
       </c>
     </row>
     <row r="183">
@@ -3165,7 +3165,7 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>1.732233125254883</v>
+        <v>2.693625292463095</v>
       </c>
     </row>
     <row r="184">
@@ -3180,7 +3180,7 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>1.087175116699698</v>
+        <v>3.198108619571732</v>
       </c>
     </row>
     <row r="185">
@@ -3195,7 +3195,7 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>3.409568107496018</v>
+        <v>1.209432827950791</v>
       </c>
     </row>
     <row r="186">
@@ -3210,7 +3210,7 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>1.727256354394729</v>
+        <v>4.630343951409607</v>
       </c>
     </row>
     <row r="187">
@@ -3225,7 +3225,7 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>4.22509463598773</v>
+        <v>3.954075030496945</v>
       </c>
     </row>
     <row r="188">
@@ -3240,7 +3240,7 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>4.427751430288921</v>
+        <v>4.989742043244445</v>
       </c>
     </row>
     <row r="189">
@@ -3255,7 +3255,7 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>3.409487930870152</v>
+        <v>1.981700049886022</v>
       </c>
     </row>
     <row r="190">
@@ -3270,7 +3270,7 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>4.456625597027005</v>
+        <v>2.92032054815556</v>
       </c>
     </row>
     <row r="191">
@@ -3285,7 +3285,7 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>2.937347358362635</v>
+        <v>2.160724686744806</v>
       </c>
     </row>
     <row r="192">
@@ -3300,7 +3300,7 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>2.848587424029814</v>
+        <v>3.77667442708656</v>
       </c>
     </row>
     <row r="193">
@@ -3315,7 +3315,7 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>3.441397224226275</v>
+        <v>3.403269785055725</v>
       </c>
     </row>
     <row r="194">
@@ -3330,7 +3330,7 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>2.660123498682993</v>
+        <v>2.208323647034642</v>
       </c>
     </row>
     <row r="195">
@@ -3345,7 +3345,7 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>4.020852852668453</v>
+        <v>4.801608837717928</v>
       </c>
     </row>
     <row r="196">
@@ -3360,7 +3360,7 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>2.588223048196586</v>
+        <v>3.063503991505826</v>
       </c>
     </row>
     <row r="197">
@@ -3375,7 +3375,7 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>3.798116353917061</v>
+        <v>3.021223531436564</v>
       </c>
     </row>
     <row r="198">
@@ -3390,7 +3390,7 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>3.974782798617006</v>
+        <v>4.513582927823853</v>
       </c>
     </row>
     <row r="199">
@@ -3405,7 +3405,7 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>4.724600486946425</v>
+        <v>1.258544961739164</v>
       </c>
     </row>
     <row r="200">
@@ -3420,7 +3420,7 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>4.478309368496644</v>
+        <v>2.067563899527792</v>
       </c>
     </row>
     <row r="201">
@@ -3435,7 +3435,7 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>4.285416070823556</v>
+        <v>1.217623457653751</v>
       </c>
     </row>
     <row r="202">
@@ -3450,7 +3450,7 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>2.141106600995158</v>
+        <v>1.172545424117545</v>
       </c>
     </row>
     <row r="203">
@@ -3465,7 +3465,7 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>4.157683157374944</v>
+        <v>3.263491764916016</v>
       </c>
     </row>
     <row r="204">
@@ -3480,7 +3480,7 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>3.018767917029338</v>
+        <v>3.371402506769767</v>
       </c>
     </row>
     <row r="205">
@@ -3495,7 +3495,7 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>4.6915863924436</v>
+        <v>3.550042380208033</v>
       </c>
     </row>
     <row r="206">
@@ -3510,7 +3510,7 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>2.047698467277359</v>
+        <v>1.515828510153328</v>
       </c>
     </row>
     <row r="207">
@@ -3525,7 +3525,7 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>3.76724959537025</v>
+        <v>4.750008421443644</v>
       </c>
     </row>
     <row r="208">
@@ -3540,7 +3540,7 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>2.222929660537248</v>
+        <v>1.808487370627359</v>
       </c>
     </row>
     <row r="209">
@@ -3555,7 +3555,7 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>3.841502741254658</v>
+        <v>3.893173355877918</v>
       </c>
     </row>
     <row r="210">
@@ -3570,7 +3570,7 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>2.440812367895761</v>
+        <v>3.216703420337204</v>
       </c>
     </row>
     <row r="211">
@@ -3585,7 +3585,7 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>2.4054032434165</v>
+        <v>1.796735777378929</v>
       </c>
     </row>
     <row r="212">
@@ -3600,7 +3600,7 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>2.024155808355762</v>
+        <v>1.045795952656897</v>
       </c>
     </row>
     <row r="213">
@@ -3615,7 +3615,7 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>3.716256392167372</v>
+        <v>2.447306965868655</v>
       </c>
     </row>
     <row r="214">
@@ -3630,7 +3630,7 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>2.303806272016513</v>
+        <v>1.240542617189077</v>
       </c>
     </row>
     <row r="215">
@@ -3645,7 +3645,7 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>3.836859368484169</v>
+        <v>3.275217987460214</v>
       </c>
     </row>
     <row r="216">
@@ -3660,7 +3660,7 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>4.361617786698226</v>
+        <v>2.617328228103652</v>
       </c>
     </row>
     <row r="217">
@@ -3675,7 +3675,7 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>4.514902352604531</v>
+        <v>3.051922324144181</v>
       </c>
     </row>
     <row r="218">
@@ -3690,7 +3690,7 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>2.663684573102132</v>
+        <v>1.732829265737565</v>
       </c>
     </row>
     <row r="219">
@@ -3705,7 +3705,7 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>2.332906542592863</v>
+        <v>2.686325259000264</v>
       </c>
     </row>
     <row r="220">
@@ -3720,7 +3720,7 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>1.926658968367832</v>
+        <v>1.017919390897376</v>
       </c>
     </row>
     <row r="221">
@@ -3735,7 +3735,7 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>2.318360276221523</v>
+        <v>3.528743181235347</v>
       </c>
     </row>
     <row r="222">
@@ -3750,7 +3750,7 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>2.170847669397425</v>
+        <v>1.699566484556942</v>
       </c>
     </row>
     <row r="223">
@@ -3765,7 +3765,7 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>3.868897031170134</v>
+        <v>3.951721151465255</v>
       </c>
     </row>
     <row r="224">
@@ -3780,7 +3780,7 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>4.982750570896888</v>
+        <v>3.579940827811344</v>
       </c>
     </row>
     <row r="225">
@@ -3795,7 +3795,7 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>1.941124410188788</v>
+        <v>2.901097892506164</v>
       </c>
     </row>
     <row r="226">
@@ -3810,7 +3810,7 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>1.812540539925255</v>
+        <v>4.622763207987869</v>
       </c>
     </row>
     <row r="227">
@@ -3825,7 +3825,7 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>1.738693047939627</v>
+        <v>3.874186485651138</v>
       </c>
     </row>
     <row r="228">
@@ -3840,7 +3840,7 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>4.302635422797539</v>
+        <v>4.878720055811463</v>
       </c>
     </row>
     <row r="229">
@@ -3855,7 +3855,7 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>4.371546631221582</v>
+        <v>1.963248070910324</v>
       </c>
     </row>
     <row r="230">
@@ -3870,7 +3870,7 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>3.908059432552115</v>
+        <v>1.582568094489003</v>
       </c>
     </row>
     <row r="231">
@@ -3885,7 +3885,7 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>1.897479428718253</v>
+        <v>1.021170249803689</v>
       </c>
     </row>
     <row r="232">
@@ -3900,7 +3900,7 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>2.587415770516317</v>
+        <v>2.977881572095577</v>
       </c>
     </row>
     <row r="233">
@@ -3915,7 +3915,7 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>4.667929058462864</v>
+        <v>2.574657085916422</v>
       </c>
     </row>
     <row r="234">
@@ -3930,7 +3930,7 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>1.90476732971167</v>
+        <v>3.486143213659599</v>
       </c>
     </row>
     <row r="235">
@@ -3945,7 +3945,7 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>2.352757892171085</v>
+        <v>2.877044198882399</v>
       </c>
     </row>
     <row r="236">
@@ -3960,7 +3960,7 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>4.488052872245463</v>
+        <v>2.131766117231346</v>
       </c>
     </row>
     <row r="237">
@@ -3975,7 +3975,7 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>2.772759565725547</v>
+        <v>4.204232017101101</v>
       </c>
     </row>
     <row r="238">
@@ -3990,7 +3990,7 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>2.029962081419091</v>
+        <v>2.871269837211799</v>
       </c>
     </row>
     <row r="239">
@@ -4005,7 +4005,7 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>2.846363514682778</v>
+        <v>4.045208652977291</v>
       </c>
     </row>
     <row r="240">
@@ -4020,7 +4020,7 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>1.93392940089027</v>
+        <v>3.34417499767867</v>
       </c>
     </row>
     <row r="241">
@@ -4035,7 +4035,7 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>2.193184320467067</v>
+        <v>2.940144821039488</v>
       </c>
     </row>
     <row r="242">
@@ -4050,7 +4050,7 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>2.426039241004212</v>
+        <v>3.222963134840583</v>
       </c>
     </row>
     <row r="243">
@@ -4065,7 +4065,7 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>2.231376945019148</v>
+        <v>3.82596000493141</v>
       </c>
     </row>
     <row r="244">
@@ -4080,7 +4080,7 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>3.184920351114603</v>
+        <v>1.81436148499981</v>
       </c>
     </row>
     <row r="245">
@@ -4095,7 +4095,7 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>3.862417613987475</v>
+        <v>2.83200584988598</v>
       </c>
     </row>
     <row r="246">
@@ -4110,7 +4110,7 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>1.632892668508477</v>
+        <v>1.118671045041855</v>
       </c>
     </row>
     <row r="247">
@@ -4125,7 +4125,7 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>1.960017323206646</v>
+        <v>3.657186250552141</v>
       </c>
     </row>
     <row r="248">
@@ -4140,7 +4140,7 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>2.53246002454047</v>
+        <v>2.681720469489549</v>
       </c>
     </row>
     <row r="249">
@@ -4155,7 +4155,7 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>4.576018429598522</v>
+        <v>1.819849900479046</v>
       </c>
     </row>
     <row r="250">
@@ -4170,7 +4170,7 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>1.531615425393163</v>
+        <v>2.556219501005093</v>
       </c>
     </row>
     <row r="251">
@@ -4185,7 +4185,7 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>3.513871752703553</v>
+        <v>3.190235045232389</v>
       </c>
     </row>
     <row r="252">
@@ -4200,7 +4200,7 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>3.594985470887737</v>
+        <v>1.496858479708362</v>
       </c>
     </row>
     <row r="253">
@@ -4215,7 +4215,7 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>1.881685497090815</v>
+        <v>2.22733312818636</v>
       </c>
     </row>
     <row r="254">
@@ -4230,7 +4230,7 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>1.809274972693482</v>
+        <v>2.082028665375475</v>
       </c>
     </row>
     <row r="255">
@@ -4245,7 +4245,7 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>1.807163507655904</v>
+        <v>1.327896806184254</v>
       </c>
     </row>
     <row r="256">
@@ -4260,7 +4260,7 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>4.893434958685621</v>
+        <v>3.134043690294071</v>
       </c>
     </row>
     <row r="257">
@@ -4275,7 +4275,7 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>1.48579626852543</v>
+        <v>1.699697714595977</v>
       </c>
     </row>
     <row r="258">
@@ -4290,7 +4290,7 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>1.088803826875644</v>
+        <v>1.966909107433501</v>
       </c>
     </row>
     <row r="259">
@@ -4305,7 +4305,7 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>4.297650880451235</v>
+        <v>4.334593684213294</v>
       </c>
     </row>
     <row r="260">
@@ -4320,7 +4320,7 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>1.094480639394213</v>
+        <v>4.442756535904154</v>
       </c>
     </row>
     <row r="261">
@@ -4335,7 +4335,7 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>4.049775381351765</v>
+        <v>4.750729907400992</v>
       </c>
     </row>
     <row r="262">
@@ -4350,7 +4350,7 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>1.215371366608282</v>
+        <v>3.266037167523321</v>
       </c>
     </row>
     <row r="263">
@@ -4365,7 +4365,7 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>2.665504814281627</v>
+        <v>4.944000344738527</v>
       </c>
     </row>
     <row r="264">
@@ -4380,7 +4380,7 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>4.381189291750681</v>
+        <v>4.9749912427535</v>
       </c>
     </row>
     <row r="265">
@@ -4395,7 +4395,7 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>4.087753846829456</v>
+        <v>4.051430683311144</v>
       </c>
     </row>
     <row r="266">
@@ -4410,7 +4410,7 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>3.530502017975125</v>
+        <v>4.024094683543728</v>
       </c>
     </row>
     <row r="267">
@@ -4425,7 +4425,7 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>2.992534285603722</v>
+        <v>3.414189571690656</v>
       </c>
     </row>
     <row r="268">
@@ -4440,7 +4440,7 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>3.737975573527626</v>
+        <v>4.822954185172651</v>
       </c>
     </row>
     <row r="269">
@@ -4455,7 +4455,7 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>1.19739840442569</v>
+        <v>2.694442198520984</v>
       </c>
     </row>
     <row r="270">
@@ -4470,7 +4470,7 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>1.700069655741643</v>
+        <v>1.285162795504512</v>
       </c>
     </row>
     <row r="271">
@@ -4485,7 +4485,7 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>4.165529839340742</v>
+        <v>1.681811547301929</v>
       </c>
     </row>
     <row r="272">
@@ -4500,7 +4500,7 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>4.359009034338658</v>
+        <v>4.304878977121618</v>
       </c>
     </row>
     <row r="273">
@@ -4515,7 +4515,7 @@
         </is>
       </c>
       <c r="C273" t="n">
-        <v>3.353300133614013</v>
+        <v>1.435108016857478</v>
       </c>
     </row>
     <row r="274">
@@ -4530,7 +4530,7 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>1.093638559827411</v>
+        <v>4.245638895935006</v>
       </c>
     </row>
     <row r="275">
@@ -4545,7 +4545,7 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>1.72700298277903</v>
+        <v>2.073758549708781</v>
       </c>
     </row>
     <row r="276">
@@ -4560,7 +4560,7 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>2.399277381001226</v>
+        <v>1.915970137130567</v>
       </c>
     </row>
     <row r="277">
@@ -4575,7 +4575,7 @@
         </is>
       </c>
       <c r="C277" t="n">
-        <v>2.93958902675295</v>
+        <v>4.795629290884647</v>
       </c>
     </row>
     <row r="278">
@@ -4590,7 +4590,7 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>2.570679523317413</v>
+        <v>2.683268941512811</v>
       </c>
     </row>
     <row r="279">
@@ -4605,7 +4605,7 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>1.238760531831919</v>
+        <v>3.600104889679333</v>
       </c>
     </row>
     <row r="280">
@@ -4620,7 +4620,7 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>1.851975163836386</v>
+        <v>4.430795279179802</v>
       </c>
     </row>
     <row r="281">
@@ -4635,7 +4635,7 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>1.271958259810374</v>
+        <v>4.138187841543074</v>
       </c>
     </row>
     <row r="282">
@@ -4650,7 +4650,7 @@
         </is>
       </c>
       <c r="C282" t="n">
-        <v>2.079778571032048</v>
+        <v>1.28284662608998</v>
       </c>
     </row>
     <row r="283">
@@ -4665,7 +4665,7 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>3.17009045217728</v>
+        <v>3.541846446656714</v>
       </c>
     </row>
     <row r="284">
@@ -4680,7 +4680,7 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>2.021973743223719</v>
+        <v>4.124737767119459</v>
       </c>
     </row>
     <row r="285">
@@ -4695,7 +4695,7 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>2.354196684527174</v>
+        <v>1.753918680156228</v>
       </c>
     </row>
     <row r="286">
@@ -4710,7 +4710,7 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>3.200858703056974</v>
+        <v>2.388551778861126</v>
       </c>
     </row>
     <row r="287">
@@ -4725,7 +4725,7 @@
         </is>
       </c>
       <c r="C287" t="n">
-        <v>4.232028500564256</v>
+        <v>3.553848498840551</v>
       </c>
     </row>
     <row r="288">
@@ -4740,7 +4740,7 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>2.252940679265293</v>
+        <v>3.227746424422121</v>
       </c>
     </row>
     <row r="289">
@@ -4755,7 +4755,7 @@
         </is>
       </c>
       <c r="C289" t="n">
-        <v>3.188688832005431</v>
+        <v>4.788914290809448</v>
       </c>
     </row>
     <row r="290">
@@ -4770,7 +4770,7 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>4.776616439427588</v>
+        <v>4.640610466453334</v>
       </c>
     </row>
     <row r="291">
@@ -4785,7 +4785,7 @@
         </is>
       </c>
       <c r="C291" t="n">
-        <v>3.833525471297508</v>
+        <v>2.601083318536032</v>
       </c>
     </row>
     <row r="292">
@@ -4800,7 +4800,7 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>2.096882436090436</v>
+        <v>2.648215784813877</v>
       </c>
     </row>
     <row r="293">
@@ -4815,7 +4815,7 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>3.695478158595169</v>
+        <v>3.885340222311822</v>
       </c>
     </row>
     <row r="294">
@@ -4830,7 +4830,7 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>4.894600735228154</v>
+        <v>2.493777298575662</v>
       </c>
     </row>
     <row r="295">
@@ -4845,7 +4845,7 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>3.021163154170039</v>
+        <v>1.520286225209204</v>
       </c>
     </row>
     <row r="296">
@@ -4860,7 +4860,7 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>2.975668975897692</v>
+        <v>2.951772220521963</v>
       </c>
     </row>
     <row r="297">
@@ -4875,7 +4875,7 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>4.236482362464196</v>
+        <v>1.599359853929329</v>
       </c>
     </row>
     <row r="298">
@@ -4890,7 +4890,7 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>4.223391593822971</v>
+        <v>1.761979320629933</v>
       </c>
     </row>
     <row r="299">
@@ -4905,7 +4905,7 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>2.421116328504504</v>
+        <v>1.55702127854358</v>
       </c>
     </row>
     <row r="300">
@@ -4920,7 +4920,7 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>1.179425659119055</v>
+        <v>2.21547862487144</v>
       </c>
     </row>
     <row r="301">
@@ -4935,7 +4935,7 @@
         </is>
       </c>
       <c r="C301" t="n">
-        <v>1.515984189549445</v>
+        <v>1.912040448459437</v>
       </c>
     </row>
     <row r="302">
@@ -4950,7 +4950,7 @@
         </is>
       </c>
       <c r="C302" t="n">
-        <v>4.052315586312863</v>
+        <v>4.996792835188819</v>
       </c>
     </row>
     <row r="303">
@@ -4965,7 +4965,7 @@
         </is>
       </c>
       <c r="C303" t="n">
-        <v>2.663667387718208</v>
+        <v>3.288739598916262</v>
       </c>
     </row>
     <row r="304">
@@ -4980,7 +4980,7 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>4.354603923743719</v>
+        <v>2.096378232301698</v>
       </c>
     </row>
     <row r="305">
@@ -4995,7 +4995,7 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>4.075252094711772</v>
+        <v>2.000931851167606</v>
       </c>
     </row>
     <row r="306">
@@ -5010,7 +5010,7 @@
         </is>
       </c>
       <c r="C306" t="n">
-        <v>4.061253447883773</v>
+        <v>2.518243747602594</v>
       </c>
     </row>
     <row r="307">
@@ -5025,7 +5025,7 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>3.194018443206022</v>
+        <v>2.850044990821891</v>
       </c>
     </row>
     <row r="308">
@@ -5040,7 +5040,7 @@
         </is>
       </c>
       <c r="C308" t="n">
-        <v>1.224346351910023</v>
+        <v>4.141901440827377</v>
       </c>
     </row>
     <row r="309">
@@ -5055,7 +5055,7 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>4.198307661312557</v>
+        <v>3.248901330415136</v>
       </c>
     </row>
     <row r="310">
@@ -5070,7 +5070,7 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>1.693206661477622</v>
+        <v>4.892580324590233</v>
       </c>
     </row>
     <row r="311">
@@ -5085,7 +5085,7 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>3.1711791686332</v>
+        <v>4.697852578114638</v>
       </c>
     </row>
     <row r="312">
@@ -5100,7 +5100,7 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>3.067057304013676</v>
+        <v>2.494651993368116</v>
       </c>
     </row>
     <row r="313">
@@ -5115,7 +5115,7 @@
         </is>
       </c>
       <c r="C313" t="n">
-        <v>3.273648162814626</v>
+        <v>2.189652716154326</v>
       </c>
     </row>
     <row r="314">
@@ -5130,7 +5130,7 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>3.113548117784664</v>
+        <v>1.030531895990025</v>
       </c>
     </row>
     <row r="315">
@@ -5145,7 +5145,7 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>3.952904348444135</v>
+        <v>1.064698780197469</v>
       </c>
     </row>
     <row r="316">
@@ -5160,7 +5160,7 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>1.764134026085392</v>
+        <v>4.645180036868335</v>
       </c>
     </row>
     <row r="317">
@@ -5175,7 +5175,7 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>1.065729234290021</v>
+        <v>3.384678356370585</v>
       </c>
     </row>
     <row r="318">
@@ -5190,7 +5190,7 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>4.335737662822018</v>
+        <v>4.636748451375615</v>
       </c>
     </row>
     <row r="319">
@@ -5205,7 +5205,7 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>2.874370699507956</v>
+        <v>1.03874149675034</v>
       </c>
     </row>
     <row r="320">
@@ -5220,7 +5220,7 @@
         </is>
       </c>
       <c r="C320" t="n">
-        <v>1.948170898915723</v>
+        <v>4.49244549892167</v>
       </c>
     </row>
     <row r="321">
@@ -5235,7 +5235,7 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>4.581246522158878</v>
+        <v>2.210477606741286</v>
       </c>
     </row>
     <row r="322">
@@ -5250,7 +5250,7 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>4.658990201890457</v>
+        <v>2.223469899346049</v>
       </c>
     </row>
     <row r="323">
@@ -5265,7 +5265,7 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>3.555984281785783</v>
+        <v>3.92523954580732</v>
       </c>
     </row>
     <row r="324">
@@ -5280,7 +5280,7 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>3.439533499859895</v>
+        <v>2.947000452715983</v>
       </c>
     </row>
     <row r="325">
@@ -5295,7 +5295,7 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>4.906074814563011</v>
+        <v>4.890449709876943</v>
       </c>
     </row>
     <row r="326">
@@ -5310,7 +5310,7 @@
         </is>
       </c>
       <c r="C326" t="n">
-        <v>2.619423206668071</v>
+        <v>2.910066160129186</v>
       </c>
     </row>
     <row r="327">
@@ -5325,7 +5325,7 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>4.796842542963004</v>
+        <v>2.619305433401934</v>
       </c>
     </row>
     <row r="328">
@@ -5340,7 +5340,7 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>1.588951464426994</v>
+        <v>4.816259301701924</v>
       </c>
     </row>
     <row r="329">
@@ -5355,7 +5355,7 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>3.189774506156077</v>
+        <v>3.190263760019388</v>
       </c>
     </row>
     <row r="330">
@@ -5370,7 +5370,7 @@
         </is>
       </c>
       <c r="C330" t="n">
-        <v>4.006573878377093</v>
+        <v>4.69072923084434</v>
       </c>
     </row>
     <row r="331">
@@ -5385,7 +5385,7 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>1.964834004872726</v>
+        <v>3.256080130573092</v>
       </c>
     </row>
     <row r="332">
@@ -5400,7 +5400,7 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>3.876799098934343</v>
+        <v>2.146040554679483</v>
       </c>
     </row>
     <row r="333">
@@ -5415,7 +5415,7 @@
         </is>
       </c>
       <c r="C333" t="n">
-        <v>4.653436909496261</v>
+        <v>1.46033881855014</v>
       </c>
     </row>
     <row r="334">
@@ -5430,7 +5430,7 @@
         </is>
       </c>
       <c r="C334" t="n">
-        <v>4.721534890659497</v>
+        <v>2.961773020012256</v>
       </c>
     </row>
     <row r="335">
@@ -5445,7 +5445,7 @@
         </is>
       </c>
       <c r="C335" t="n">
-        <v>1.843080191985868</v>
+        <v>4.643220317501975</v>
       </c>
     </row>
     <row r="336">
@@ -5460,7 +5460,7 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>4.710250691791961</v>
+        <v>1.63008931829339</v>
       </c>
     </row>
     <row r="337">
@@ -5475,7 +5475,7 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>1.943627668806487</v>
+        <v>1.754704358269009</v>
       </c>
     </row>
     <row r="338">
@@ -5490,7 +5490,7 @@
         </is>
       </c>
       <c r="C338" t="n">
-        <v>1.660810234608202</v>
+        <v>2.001610040308186</v>
       </c>
     </row>
     <row r="339">
@@ -5505,7 +5505,7 @@
         </is>
       </c>
       <c r="C339" t="n">
-        <v>3.742450488711095</v>
+        <v>2.368669007528902</v>
       </c>
     </row>
     <row r="340">
@@ -5520,7 +5520,7 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>1.753290166816079</v>
+        <v>1.171118988265599</v>
       </c>
     </row>
     <row r="341">
@@ -5535,7 +5535,7 @@
         </is>
       </c>
       <c r="C341" t="n">
-        <v>2.349018665784201</v>
+        <v>1.95724318815869</v>
       </c>
     </row>
     <row r="342">
@@ -5550,7 +5550,7 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>1.333952901558999</v>
+        <v>3.333097505388479</v>
       </c>
     </row>
     <row r="343">
@@ -5565,7 +5565,7 @@
         </is>
       </c>
       <c r="C343" t="n">
-        <v>1.054299386558889</v>
+        <v>3.591885067898284</v>
       </c>
     </row>
     <row r="344">
@@ -5580,7 +5580,7 @@
         </is>
       </c>
       <c r="C344" t="n">
-        <v>4.585945628195251</v>
+        <v>4.289911547651947</v>
       </c>
     </row>
     <row r="345">
@@ -5595,7 +5595,7 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>4.484724253092361</v>
+        <v>1.737157901714968</v>
       </c>
     </row>
     <row r="346">
@@ -5610,7 +5610,7 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>4.282723133393334</v>
+        <v>3.925150111180674</v>
       </c>
     </row>
     <row r="347">
@@ -5625,7 +5625,7 @@
         </is>
       </c>
       <c r="C347" t="n">
-        <v>1.926115142135699</v>
+        <v>4.03374129956833</v>
       </c>
     </row>
     <row r="348">
@@ -5640,7 +5640,7 @@
         </is>
       </c>
       <c r="C348" t="n">
-        <v>1.026315400526723</v>
+        <v>1.5316335008736</v>
       </c>
     </row>
     <row r="349">
@@ -5655,7 +5655,7 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>2.438348933038092</v>
+        <v>3.736591193078985</v>
       </c>
     </row>
     <row r="350">
@@ -5670,7 +5670,7 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>4.892061148451324</v>
+        <v>3.285473536906948</v>
       </c>
     </row>
     <row r="351">
@@ -5685,7 +5685,7 @@
         </is>
       </c>
       <c r="C351" t="n">
-        <v>4.814165295547868</v>
+        <v>3.409009644561985</v>
       </c>
     </row>
     <row r="352">
@@ -5700,7 +5700,7 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>1.801002843719839</v>
+        <v>3.022504854890096</v>
       </c>
     </row>
     <row r="353">
@@ -5715,7 +5715,7 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>4.832218457233946</v>
+        <v>2.046690507349052</v>
       </c>
     </row>
     <row r="354">
@@ -5730,7 +5730,7 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>1.25493922065934</v>
+        <v>4.975031760780242</v>
       </c>
     </row>
     <row r="355">
@@ -5745,7 +5745,7 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>1.820955172778614</v>
+        <v>1.234532837391847</v>
       </c>
     </row>
     <row r="356">
@@ -5760,7 +5760,7 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>4.392104433859165</v>
+        <v>2.447660386300686</v>
       </c>
     </row>
     <row r="357">
@@ -5775,7 +5775,7 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>3.283612339354488</v>
+        <v>4.964732496787489</v>
       </c>
     </row>
     <row r="358">
@@ -5790,7 +5790,7 @@
         </is>
       </c>
       <c r="C358" t="n">
-        <v>1.382951187732997</v>
+        <v>4.220814141561828</v>
       </c>
     </row>
     <row r="359">
@@ -5805,7 +5805,7 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>1.214948249057599</v>
+        <v>2.129682132965707</v>
       </c>
     </row>
     <row r="360">
@@ -5820,7 +5820,7 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>4.648524282263559</v>
+        <v>3.073383541599711</v>
       </c>
     </row>
     <row r="361">
@@ -5835,7 +5835,7 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>4.189595588280733</v>
+        <v>4.641275086330886</v>
       </c>
     </row>
     <row r="362">
@@ -5850,7 +5850,7 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>4.272757740037889</v>
+        <v>2.483055552684311</v>
       </c>
     </row>
     <row r="363">
@@ -5865,7 +5865,7 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>2.535646507187895</v>
+        <v>2.781349342961074</v>
       </c>
     </row>
     <row r="364">
@@ -5880,7 +5880,7 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>1.779538117846461</v>
+        <v>2.030185268522156</v>
       </c>
     </row>
     <row r="365">
@@ -5895,7 +5895,7 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>4.123467555433025</v>
+        <v>4.24529523775038</v>
       </c>
     </row>
     <row r="366">
@@ -5910,7 +5910,7 @@
         </is>
       </c>
       <c r="C366" t="n">
-        <v>3.700879316328159</v>
+        <v>1.296599995241477</v>
       </c>
     </row>
     <row r="367">
@@ -5925,7 +5925,7 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>4.86771459785101</v>
+        <v>1.716744917071515</v>
       </c>
     </row>
     <row r="368">
@@ -5940,7 +5940,7 @@
         </is>
       </c>
       <c r="C368" t="n">
-        <v>2.960983021632292</v>
+        <v>2.377445307156592</v>
       </c>
     </row>
     <row r="369">
@@ -5955,7 +5955,7 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>1.405422826090659</v>
+        <v>4.767685482005547</v>
       </c>
     </row>
     <row r="370">
@@ -5970,7 +5970,7 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>4.643962678126467</v>
+        <v>3.309677090640387</v>
       </c>
     </row>
     <row r="371">
@@ -5985,7 +5985,7 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>3.448718654391739</v>
+        <v>3.461994666114462</v>
       </c>
     </row>
     <row r="372">
@@ -6000,7 +6000,7 @@
         </is>
       </c>
       <c r="C372" t="n">
-        <v>1.831161193197334</v>
+        <v>4.579600089305688</v>
       </c>
     </row>
     <row r="373">
@@ -6015,7 +6015,7 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>4.894230370501592</v>
+        <v>1.47863627309348</v>
       </c>
     </row>
     <row r="374">
@@ -6030,7 +6030,7 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>2.989276645350416</v>
+        <v>1.156892919081935</v>
       </c>
     </row>
     <row r="375">
@@ -6045,7 +6045,7 @@
         </is>
       </c>
       <c r="C375" t="n">
-        <v>3.162732847835097</v>
+        <v>1.677726487467073</v>
       </c>
     </row>
     <row r="376">
@@ -6060,7 +6060,7 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>3.221125536079555</v>
+        <v>1.917416666636545</v>
       </c>
     </row>
     <row r="377">
@@ -6075,7 +6075,7 @@
         </is>
       </c>
       <c r="C377" t="n">
-        <v>4.875063838015611</v>
+        <v>1.614227851025866</v>
       </c>
     </row>
     <row r="378">
@@ -6090,7 +6090,7 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>3.03277629161848</v>
+        <v>1.332874919717479</v>
       </c>
     </row>
     <row r="379">
@@ -6105,7 +6105,7 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>3.379057561766744</v>
+        <v>1.857895893930611</v>
       </c>
     </row>
     <row r="380">
@@ -6120,7 +6120,7 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>2.759056628212136</v>
+        <v>2.762013371467364</v>
       </c>
     </row>
     <row r="381">
@@ -6135,7 +6135,7 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>4.952024801434209</v>
+        <v>3.43815536303348</v>
       </c>
     </row>
     <row r="382">
@@ -6150,7 +6150,7 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>3.026352117536506</v>
+        <v>3.119670888447872</v>
       </c>
     </row>
     <row r="383">
@@ -6165,7 +6165,7 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>3.355626643982225</v>
+        <v>1.35501635209737</v>
       </c>
     </row>
     <row r="384">
@@ -6180,7 +6180,7 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>4.494532756077008</v>
+        <v>1.389181064045803</v>
       </c>
     </row>
     <row r="385">
@@ -6195,7 +6195,7 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>2.684016771937359</v>
+        <v>2.255353458301116</v>
       </c>
     </row>
     <row r="386">
@@ -6210,7 +6210,7 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>4.684781839180207</v>
+        <v>3.623095568343742</v>
       </c>
     </row>
     <row r="387">
@@ -6225,7 +6225,7 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>1.881448444239365</v>
+        <v>4.33215968344728</v>
       </c>
     </row>
     <row r="388">
@@ -6240,7 +6240,7 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>4.976843958055222</v>
+        <v>1.255643005284067</v>
       </c>
     </row>
     <row r="389">
@@ -6255,7 +6255,7 @@
         </is>
       </c>
       <c r="C389" t="n">
-        <v>4.260512714168583</v>
+        <v>2.324746560183104</v>
       </c>
     </row>
     <row r="390">
@@ -6270,7 +6270,7 @@
         </is>
       </c>
       <c r="C390" t="n">
-        <v>1.28717748713586</v>
+        <v>3.372618704699084</v>
       </c>
     </row>
     <row r="391">
@@ -6285,7 +6285,7 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>3.053090976559145</v>
+        <v>4.353660422148888</v>
       </c>
     </row>
     <row r="392">
@@ -6300,7 +6300,7 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>1.574166114768146</v>
+        <v>2.781989405158899</v>
       </c>
     </row>
     <row r="393">
@@ -6315,7 +6315,7 @@
         </is>
       </c>
       <c r="C393" t="n">
-        <v>4.240407956849801</v>
+        <v>3.745103472791355</v>
       </c>
     </row>
     <row r="394">
@@ -6330,7 +6330,7 @@
         </is>
       </c>
       <c r="C394" t="n">
-        <v>4.126445382852395</v>
+        <v>1.302125637770815</v>
       </c>
     </row>
     <row r="395">
@@ -6345,7 +6345,7 @@
         </is>
       </c>
       <c r="C395" t="n">
-        <v>3.19066083495479</v>
+        <v>4.073858963930472</v>
       </c>
     </row>
     <row r="396">
@@ -6360,7 +6360,7 @@
         </is>
       </c>
       <c r="C396" t="n">
-        <v>4.113272414549463</v>
+        <v>4.555679490446376</v>
       </c>
     </row>
     <row r="397">
@@ -6375,7 +6375,7 @@
         </is>
       </c>
       <c r="C397" t="n">
-        <v>4.693573349119054</v>
+        <v>2.106346262868001</v>
       </c>
     </row>
     <row r="398">
@@ -6390,7 +6390,7 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>3.817787245479448</v>
+        <v>1.964836245103041</v>
       </c>
     </row>
     <row r="399">
@@ -6405,7 +6405,7 @@
         </is>
       </c>
       <c r="C399" t="n">
-        <v>1.443905420615915</v>
+        <v>1.223379947609904</v>
       </c>
     </row>
     <row r="400">
@@ -6420,7 +6420,7 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>2.362824619617653</v>
+        <v>4.657197548108691</v>
       </c>
     </row>
     <row r="401">
@@ -6435,7 +6435,7 @@
         </is>
       </c>
       <c r="C401" t="n">
-        <v>2.792156695579931</v>
+        <v>3.503274912359424</v>
       </c>
     </row>
     <row r="402">
@@ -6450,7 +6450,7 @@
         </is>
       </c>
       <c r="C402" t="n">
-        <v>3.916560784635577</v>
+        <v>1.556804810972719</v>
       </c>
     </row>
     <row r="403">
@@ -6465,7 +6465,7 @@
         </is>
       </c>
       <c r="C403" t="n">
-        <v>2.215414706708546</v>
+        <v>4.349351435185718</v>
       </c>
     </row>
     <row r="404">
@@ -6480,7 +6480,7 @@
         </is>
       </c>
       <c r="C404" t="n">
-        <v>4.502581274205093</v>
+        <v>3.42577284602541</v>
       </c>
     </row>
     <row r="405">
@@ -6495,7 +6495,7 @@
         </is>
       </c>
       <c r="C405" t="n">
-        <v>1.284618219250123</v>
+        <v>2.213645335616551</v>
       </c>
     </row>
     <row r="406">
@@ -6510,7 +6510,7 @@
         </is>
       </c>
       <c r="C406" t="n">
-        <v>4.002508873898501</v>
+        <v>2.177165814763046</v>
       </c>
     </row>
     <row r="407">
@@ -6525,7 +6525,7 @@
         </is>
       </c>
       <c r="C407" t="n">
-        <v>3.335357060546297</v>
+        <v>4.82645081425578</v>
       </c>
     </row>
     <row r="408">
@@ -6540,7 +6540,7 @@
         </is>
       </c>
       <c r="C408" t="n">
-        <v>2.394093429194897</v>
+        <v>1.318258920411104</v>
       </c>
     </row>
     <row r="409">
@@ -6555,7 +6555,7 @@
         </is>
       </c>
       <c r="C409" t="n">
-        <v>1.228805555164684</v>
+        <v>4.347446945789207</v>
       </c>
     </row>
     <row r="410">
@@ -6570,7 +6570,7 @@
         </is>
       </c>
       <c r="C410" t="n">
-        <v>3.532325323388199</v>
+        <v>1.67996295874487</v>
       </c>
     </row>
     <row r="411">
@@ -6585,7 +6585,7 @@
         </is>
       </c>
       <c r="C411" t="n">
-        <v>3.640199840640479</v>
+        <v>3.390670899858514</v>
       </c>
     </row>
     <row r="412">
@@ -6600,7 +6600,7 @@
         </is>
       </c>
       <c r="C412" t="n">
-        <v>4.408541565068798</v>
+        <v>3.775852614916359</v>
       </c>
     </row>
     <row r="413">
@@ -6615,7 +6615,7 @@
         </is>
       </c>
       <c r="C413" t="n">
-        <v>1.593573673872445</v>
+        <v>1.126485744302445</v>
       </c>
     </row>
     <row r="414">
@@ -6630,7 +6630,7 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>1.861294270549755</v>
+        <v>2.421665793370311</v>
       </c>
     </row>
     <row r="415">
@@ -6645,7 +6645,7 @@
         </is>
       </c>
       <c r="C415" t="n">
-        <v>2.405567587230764</v>
+        <v>4.350096992036113</v>
       </c>
     </row>
     <row r="416">
@@ -6660,7 +6660,7 @@
         </is>
       </c>
       <c r="C416" t="n">
-        <v>1.608580976920445</v>
+        <v>2.472880968168277</v>
       </c>
     </row>
     <row r="417">
@@ -6675,7 +6675,7 @@
         </is>
       </c>
       <c r="C417" t="n">
-        <v>3.592768175549398</v>
+        <v>3.79306646334926</v>
       </c>
     </row>
     <row r="418">
@@ -6690,7 +6690,7 @@
         </is>
       </c>
       <c r="C418" t="n">
-        <v>3.482509125461912</v>
+        <v>1.342139311662982</v>
       </c>
     </row>
     <row r="419">
@@ -6705,7 +6705,7 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>1.370196050284249</v>
+        <v>2.618578318410049</v>
       </c>
     </row>
     <row r="420">
@@ -6720,7 +6720,7 @@
         </is>
       </c>
       <c r="C420" t="n">
-        <v>2.652241133957498</v>
+        <v>4.867409415752391</v>
       </c>
     </row>
     <row r="421">
@@ -6735,7 +6735,7 @@
         </is>
       </c>
       <c r="C421" t="n">
-        <v>4.743942458152266</v>
+        <v>1.46851610648536</v>
       </c>
     </row>
     <row r="422">
@@ -6750,7 +6750,7 @@
         </is>
       </c>
       <c r="C422" t="n">
-        <v>3.013257435041246</v>
+        <v>1.631729704929923</v>
       </c>
     </row>
     <row r="423">
@@ -6765,7 +6765,7 @@
         </is>
       </c>
       <c r="C423" t="n">
-        <v>2.537648479200768</v>
+        <v>1.492815889479005</v>
       </c>
     </row>
     <row r="424">
@@ -6780,7 +6780,7 @@
         </is>
       </c>
       <c r="C424" t="n">
-        <v>1.362059664255582</v>
+        <v>4.714870121366664</v>
       </c>
     </row>
     <row r="425">
@@ -6795,7 +6795,7 @@
         </is>
       </c>
       <c r="C425" t="n">
-        <v>2.422007162104184</v>
+        <v>1.2039226156648</v>
       </c>
     </row>
     <row r="426">
@@ -6810,7 +6810,7 @@
         </is>
       </c>
       <c r="C426" t="n">
-        <v>1.788692425521293</v>
+        <v>3.138440302258767</v>
       </c>
     </row>
     <row r="427">
@@ -6825,7 +6825,7 @@
         </is>
       </c>
       <c r="C427" t="n">
-        <v>4.124569909949991</v>
+        <v>4.662960400094573</v>
       </c>
     </row>
     <row r="428">
@@ -6840,7 +6840,7 @@
         </is>
       </c>
       <c r="C428" t="n">
-        <v>3.39510805229393</v>
+        <v>3.051331794052596</v>
       </c>
     </row>
     <row r="429">
@@ -6855,7 +6855,7 @@
         </is>
       </c>
       <c r="C429" t="n">
-        <v>1.313635831182603</v>
+        <v>4.19661895260047</v>
       </c>
     </row>
     <row r="430">
@@ -6870,7 +6870,7 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>3.18841077923315</v>
+        <v>1.928812821578311</v>
       </c>
     </row>
     <row r="431">
@@ -6885,7 +6885,7 @@
         </is>
       </c>
       <c r="C431" t="n">
-        <v>4.782751666742078</v>
+        <v>2.381890859876313</v>
       </c>
     </row>
     <row r="432">
@@ -6900,7 +6900,7 @@
         </is>
       </c>
       <c r="C432" t="n">
-        <v>4.091195024978028</v>
+        <v>4.68791865649021</v>
       </c>
     </row>
     <row r="433">
@@ -6915,7 +6915,7 @@
         </is>
       </c>
       <c r="C433" t="n">
-        <v>1.129704410802817</v>
+        <v>3.791393633547742</v>
       </c>
     </row>
     <row r="434">
@@ -6930,7 +6930,7 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>1.066600373781224</v>
+        <v>4.323048087368432</v>
       </c>
     </row>
     <row r="435">
@@ -6945,7 +6945,7 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>2.834657695536805</v>
+        <v>1.50140844857935</v>
       </c>
     </row>
     <row r="436">
@@ -6960,7 +6960,7 @@
         </is>
       </c>
       <c r="C436" t="n">
-        <v>3.751324837089914</v>
+        <v>3.017041464678072</v>
       </c>
     </row>
     <row r="437">
@@ -6975,7 +6975,7 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>4.610922561640463</v>
+        <v>2.161618637576504</v>
       </c>
     </row>
     <row r="438">
@@ -6990,7 +6990,7 @@
         </is>
       </c>
       <c r="C438" t="n">
-        <v>1.602782661875732</v>
+        <v>4.60603433647616</v>
       </c>
     </row>
     <row r="439">
@@ -7005,7 +7005,7 @@
         </is>
       </c>
       <c r="C439" t="n">
-        <v>4.392253283179111</v>
+        <v>2.438543746235251</v>
       </c>
     </row>
     <row r="440">
@@ -7020,7 +7020,7 @@
         </is>
       </c>
       <c r="C440" t="n">
-        <v>4.824801674844435</v>
+        <v>4.464126808303338</v>
       </c>
     </row>
     <row r="441">
@@ -7035,7 +7035,7 @@
         </is>
       </c>
       <c r="C441" t="n">
-        <v>3.671379509982071</v>
+        <v>2.801919921027499</v>
       </c>
     </row>
     <row r="442">
@@ -7050,7 +7050,7 @@
         </is>
       </c>
       <c r="C442" t="n">
-        <v>4.878807924615445</v>
+        <v>4.727089600755168</v>
       </c>
     </row>
     <row r="443">
@@ -7065,7 +7065,7 @@
         </is>
       </c>
       <c r="C443" t="n">
-        <v>3.176549208398404</v>
+        <v>1.239708142935112</v>
       </c>
     </row>
     <row r="444">
@@ -7080,7 +7080,7 @@
         </is>
       </c>
       <c r="C444" t="n">
-        <v>2.163270199770689</v>
+        <v>4.377929380993065</v>
       </c>
     </row>
     <row r="445">
@@ -7095,7 +7095,7 @@
         </is>
       </c>
       <c r="C445" t="n">
-        <v>2.261745962421291</v>
+        <v>4.868161928818127</v>
       </c>
     </row>
     <row r="446">
@@ -7110,7 +7110,7 @@
         </is>
       </c>
       <c r="C446" t="n">
-        <v>2.320895307974105</v>
+        <v>2.680496358770911</v>
       </c>
     </row>
     <row r="447">
@@ -7125,7 +7125,7 @@
         </is>
       </c>
       <c r="C447" t="n">
-        <v>2.994538260857519</v>
+        <v>2.582745972612132</v>
       </c>
     </row>
     <row r="448">
@@ -7140,7 +7140,7 @@
         </is>
       </c>
       <c r="C448" t="n">
-        <v>4.782077417437758</v>
+        <v>1.349031426781431</v>
       </c>
     </row>
     <row r="449">
@@ -7155,7 +7155,7 @@
         </is>
       </c>
       <c r="C449" t="n">
-        <v>4.926020949620279</v>
+        <v>3.368025585075126</v>
       </c>
     </row>
     <row r="450">
@@ -7170,7 +7170,7 @@
         </is>
       </c>
       <c r="C450" t="n">
-        <v>2.663930430814013</v>
+        <v>4.312526848565892</v>
       </c>
     </row>
     <row r="451">
@@ -7185,7 +7185,7 @@
         </is>
       </c>
       <c r="C451" t="n">
-        <v>4.472073184322217</v>
+        <v>4.757728728226272</v>
       </c>
     </row>
     <row r="452">
@@ -7200,7 +7200,7 @@
         </is>
       </c>
       <c r="C452" t="n">
-        <v>1.480606279910857</v>
+        <v>4.842898140779221</v>
       </c>
     </row>
     <row r="453">
@@ -7215,7 +7215,7 @@
         </is>
       </c>
       <c r="C453" t="n">
-        <v>2.290294772922507</v>
+        <v>3.02240891684129</v>
       </c>
     </row>
     <row r="454">
@@ -7230,7 +7230,7 @@
         </is>
       </c>
       <c r="C454" t="n">
-        <v>4.809338087642598</v>
+        <v>3.53534261802265</v>
       </c>
     </row>
     <row r="455">
@@ -7245,7 +7245,7 @@
         </is>
       </c>
       <c r="C455" t="n">
-        <v>2.016748333014069</v>
+        <v>1.885339602931617</v>
       </c>
     </row>
     <row r="456">
@@ -7260,7 +7260,7 @@
         </is>
       </c>
       <c r="C456" t="n">
-        <v>4.76777372657768</v>
+        <v>4.96054209398444</v>
       </c>
     </row>
     <row r="457">
@@ -7275,7 +7275,7 @@
         </is>
       </c>
       <c r="C457" t="n">
-        <v>4.245148701399131</v>
+        <v>2.778488732021494</v>
       </c>
     </row>
     <row r="458">
@@ -7290,7 +7290,7 @@
         </is>
       </c>
       <c r="C458" t="n">
-        <v>3.115947114686802</v>
+        <v>3.112759851614077</v>
       </c>
     </row>
     <row r="459">
@@ -7305,7 +7305,7 @@
         </is>
       </c>
       <c r="C459" t="n">
-        <v>1.447499596048464</v>
+        <v>2.524695084277169</v>
       </c>
     </row>
     <row r="460">
@@ -7320,7 +7320,7 @@
         </is>
       </c>
       <c r="C460" t="n">
-        <v>3.803445188963584</v>
+        <v>4.506691914145025</v>
       </c>
     </row>
     <row r="461">
@@ -7335,7 +7335,7 @@
         </is>
       </c>
       <c r="C461" t="n">
-        <v>1.280797100319324</v>
+        <v>4.405746540918702</v>
       </c>
     </row>
     <row r="462">
@@ -7350,7 +7350,7 @@
         </is>
       </c>
       <c r="C462" t="n">
-        <v>2.497244872706772</v>
+        <v>1.578467879977901</v>
       </c>
     </row>
     <row r="463">
@@ -7365,7 +7365,7 @@
         </is>
       </c>
       <c r="C463" t="n">
-        <v>3.479704960665789</v>
+        <v>4.629774951440838</v>
       </c>
     </row>
     <row r="464">
@@ -7380,7 +7380,7 @@
         </is>
       </c>
       <c r="C464" t="n">
-        <v>2.964459496452576</v>
+        <v>4.831175038634107</v>
       </c>
     </row>
     <row r="465">
@@ -7395,7 +7395,7 @@
         </is>
       </c>
       <c r="C465" t="n">
-        <v>1.431426862332163</v>
+        <v>4.435760195039923</v>
       </c>
     </row>
     <row r="466">
@@ -7410,7 +7410,7 @@
         </is>
       </c>
       <c r="C466" t="n">
-        <v>1.943136963403562</v>
+        <v>1.224442213022414</v>
       </c>
     </row>
     <row r="467">
@@ -7425,7 +7425,7 @@
         </is>
       </c>
       <c r="C467" t="n">
-        <v>1.865159617656607</v>
+        <v>3.923121884652537</v>
       </c>
     </row>
     <row r="468">
@@ -7440,7 +7440,7 @@
         </is>
       </c>
       <c r="C468" t="n">
-        <v>3.247399394415643</v>
+        <v>1.8359092327738</v>
       </c>
     </row>
     <row r="469">
@@ -7455,7 +7455,7 @@
         </is>
       </c>
       <c r="C469" t="n">
-        <v>4.088501120891689</v>
+        <v>1.621169969584178</v>
       </c>
     </row>
     <row r="470">
@@ -7470,7 +7470,7 @@
         </is>
       </c>
       <c r="C470" t="n">
-        <v>2.771047364974135</v>
+        <v>1.932492999058751</v>
       </c>
     </row>
     <row r="471">
@@ -7485,7 +7485,7 @@
         </is>
       </c>
       <c r="C471" t="n">
-        <v>2.777189039092873</v>
+        <v>2.897275395058017</v>
       </c>
     </row>
     <row r="472">
@@ -7500,7 +7500,7 @@
         </is>
       </c>
       <c r="C472" t="n">
-        <v>3.072716184560742</v>
+        <v>4.276561374777161</v>
       </c>
     </row>
     <row r="473">
@@ -7515,7 +7515,7 @@
         </is>
       </c>
       <c r="C473" t="n">
-        <v>1.407033256847678</v>
+        <v>2.351008826067566</v>
       </c>
     </row>
     <row r="474">
@@ -7530,7 +7530,7 @@
         </is>
       </c>
       <c r="C474" t="n">
-        <v>2.690165286595718</v>
+        <v>4.123058380565303</v>
       </c>
     </row>
     <row r="475">
@@ -7545,7 +7545,7 @@
         </is>
       </c>
       <c r="C475" t="n">
-        <v>1.608954205060714</v>
+        <v>1.203586505041496</v>
       </c>
     </row>
     <row r="476">
@@ -7560,7 +7560,7 @@
         </is>
       </c>
       <c r="C476" t="n">
-        <v>4.552964835146488</v>
+        <v>1.56163119029898</v>
       </c>
     </row>
     <row r="477">
@@ -7575,7 +7575,7 @@
         </is>
       </c>
       <c r="C477" t="n">
-        <v>2.730718354130911</v>
+        <v>3.174340410162307</v>
       </c>
     </row>
     <row r="478">
@@ -7590,7 +7590,7 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>3.67291049752358</v>
+        <v>2.545693017144782</v>
       </c>
     </row>
     <row r="479">
@@ -7605,7 +7605,7 @@
         </is>
       </c>
       <c r="C479" t="n">
-        <v>3.946849567418205</v>
+        <v>4.563023031050717</v>
       </c>
     </row>
     <row r="480">
@@ -7620,7 +7620,7 @@
         </is>
       </c>
       <c r="C480" t="n">
-        <v>3.367812754973453</v>
+        <v>1.268124508833281</v>
       </c>
     </row>
     <row r="481">
@@ -7635,7 +7635,7 @@
         </is>
       </c>
       <c r="C481" t="n">
-        <v>1.451166195329872</v>
+        <v>2.100921311332325</v>
       </c>
     </row>
     <row r="482">
@@ -7650,7 +7650,7 @@
         </is>
       </c>
       <c r="C482" t="n">
-        <v>3.968787083329445</v>
+        <v>3.116115807488158</v>
       </c>
     </row>
     <row r="483">
@@ -7665,7 +7665,7 @@
         </is>
       </c>
       <c r="C483" t="n">
-        <v>1.499268701936682</v>
+        <v>4.860711250068704</v>
       </c>
     </row>
     <row r="484">
@@ -7680,7 +7680,7 @@
         </is>
       </c>
       <c r="C484" t="n">
-        <v>4.217425842747131</v>
+        <v>1.94630176370267</v>
       </c>
     </row>
     <row r="485">
@@ -7695,7 +7695,7 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>4.294885107256463</v>
+        <v>4.634491148406765</v>
       </c>
     </row>
     <row r="486">
@@ -7710,7 +7710,7 @@
         </is>
       </c>
       <c r="C486" t="n">
-        <v>4.385595858182235</v>
+        <v>2.322011841422811</v>
       </c>
     </row>
     <row r="487">
@@ -7725,7 +7725,7 @@
         </is>
       </c>
       <c r="C487" t="n">
-        <v>3.770933124923404</v>
+        <v>4.350622420455018</v>
       </c>
     </row>
     <row r="488">
@@ -7740,7 +7740,7 @@
         </is>
       </c>
       <c r="C488" t="n">
-        <v>1.912984380424295</v>
+        <v>4.67610271149708</v>
       </c>
     </row>
     <row r="489">
@@ -7755,7 +7755,7 @@
         </is>
       </c>
       <c r="C489" t="n">
-        <v>2.84906530273938</v>
+        <v>3.326370338235653</v>
       </c>
     </row>
     <row r="490">
@@ -7770,7 +7770,7 @@
         </is>
       </c>
       <c r="C490" t="n">
-        <v>2.643395246838884</v>
+        <v>4.417685525657786</v>
       </c>
     </row>
     <row r="491">
@@ -7785,7 +7785,7 @@
         </is>
       </c>
       <c r="C491" t="n">
-        <v>1.465412965498302</v>
+        <v>2.194589941340042</v>
       </c>
     </row>
     <row r="492">
@@ -7800,7 +7800,7 @@
         </is>
       </c>
       <c r="C492" t="n">
-        <v>4.517690897563376</v>
+        <v>1.579663621788007</v>
       </c>
     </row>
     <row r="493">
@@ -7815,7 +7815,7 @@
         </is>
       </c>
       <c r="C493" t="n">
-        <v>3.617313360412895</v>
+        <v>3.32144318853382</v>
       </c>
     </row>
     <row r="494">
@@ -7830,7 +7830,7 @@
         </is>
       </c>
       <c r="C494" t="n">
-        <v>1.954628662790433</v>
+        <v>3.920203885728648</v>
       </c>
     </row>
     <row r="495">
@@ -7845,7 +7845,7 @@
         </is>
       </c>
       <c r="C495" t="n">
-        <v>2.296304395195495</v>
+        <v>1.34936966528229</v>
       </c>
     </row>
     <row r="496">
@@ -7860,7 +7860,7 @@
         </is>
       </c>
       <c r="C496" t="n">
-        <v>4.251592988890222</v>
+        <v>1.345395070895497</v>
       </c>
     </row>
     <row r="497">
@@ -7875,7 +7875,7 @@
         </is>
       </c>
       <c r="C497" t="n">
-        <v>4.409089890418081</v>
+        <v>2.865580729753572</v>
       </c>
     </row>
     <row r="498">
@@ -7890,7 +7890,7 @@
         </is>
       </c>
       <c r="C498" t="n">
-        <v>1.948615389036597</v>
+        <v>2.669770950846869</v>
       </c>
     </row>
     <row r="499">
@@ -7905,7 +7905,7 @@
         </is>
       </c>
       <c r="C499" t="n">
-        <v>4.683336974436305</v>
+        <v>2.677754727219802</v>
       </c>
     </row>
     <row r="500">
@@ -7920,7 +7920,7 @@
         </is>
       </c>
       <c r="C500" t="n">
-        <v>4.570726121692774</v>
+        <v>4.364088871419175</v>
       </c>
     </row>
     <row r="501">
@@ -7935,7 +7935,7 @@
         </is>
       </c>
       <c r="C501" t="n">
-        <v>2.042418236786993</v>
+        <v>2.780211647335539</v>
       </c>
     </row>
     <row r="502">
@@ -7950,7 +7950,7 @@
         </is>
       </c>
       <c r="C502" t="n">
-        <v>1.268616395180608</v>
+        <v>2.362492825055292</v>
       </c>
     </row>
     <row r="503">
@@ -7965,7 +7965,7 @@
         </is>
       </c>
       <c r="C503" t="n">
-        <v>4.279049934746896</v>
+        <v>3.448504932996275</v>
       </c>
     </row>
     <row r="504">
@@ -7980,7 +7980,7 @@
         </is>
       </c>
       <c r="C504" t="n">
-        <v>3.693016295990206</v>
+        <v>3.958527957691035</v>
       </c>
     </row>
     <row r="505">
@@ -7995,7 +7995,7 @@
         </is>
       </c>
       <c r="C505" t="n">
-        <v>3.829892252913093</v>
+        <v>2.383038633636647</v>
       </c>
     </row>
     <row r="506">
@@ -8010,7 +8010,7 @@
         </is>
       </c>
       <c r="C506" t="n">
-        <v>1.955724590637779</v>
+        <v>2.912189431076496</v>
       </c>
     </row>
     <row r="507">
@@ -8025,7 +8025,7 @@
         </is>
       </c>
       <c r="C507" t="n">
-        <v>4.907123515240373</v>
+        <v>1.895489279554625</v>
       </c>
     </row>
     <row r="508">
@@ -8040,7 +8040,7 @@
         </is>
       </c>
       <c r="C508" t="n">
-        <v>1.134036085874595</v>
+        <v>1.509426008431826</v>
       </c>
     </row>
     <row r="509">
@@ -8055,7 +8055,7 @@
         </is>
       </c>
       <c r="C509" t="n">
-        <v>4.097373920750418</v>
+        <v>3.030957251303569</v>
       </c>
     </row>
     <row r="510">
@@ -8070,7 +8070,7 @@
         </is>
       </c>
       <c r="C510" t="n">
-        <v>1.684539103375111</v>
+        <v>4.393583716383478</v>
       </c>
     </row>
     <row r="511">
@@ -8085,7 +8085,7 @@
         </is>
       </c>
       <c r="C511" t="n">
-        <v>3.565453309603897</v>
+        <v>3.263084712812839</v>
       </c>
     </row>
     <row r="512">
@@ -8100,7 +8100,7 @@
         </is>
       </c>
       <c r="C512" t="n">
-        <v>2.564015011041408</v>
+        <v>1.819428920467533</v>
       </c>
     </row>
     <row r="513">
@@ -8115,7 +8115,7 @@
         </is>
       </c>
       <c r="C513" t="n">
-        <v>4.603936704798484</v>
+        <v>4.369134991418628</v>
       </c>
     </row>
     <row r="514">
@@ -8130,7 +8130,7 @@
         </is>
       </c>
       <c r="C514" t="n">
-        <v>2.602811707782645</v>
+        <v>4.529406733767136</v>
       </c>
     </row>
     <row r="515">
@@ -8145,7 +8145,7 @@
         </is>
       </c>
       <c r="C515" t="n">
-        <v>1.15410806813893</v>
+        <v>2.032213847390713</v>
       </c>
     </row>
     <row r="516">
@@ -8160,7 +8160,7 @@
         </is>
       </c>
       <c r="C516" t="n">
-        <v>4.730268515020015</v>
+        <v>3.71620572392637</v>
       </c>
     </row>
     <row r="517">
@@ -8175,7 +8175,7 @@
         </is>
       </c>
       <c r="C517" t="n">
-        <v>1.295422481218919</v>
+        <v>4.596117588764615</v>
       </c>
     </row>
     <row r="518">
@@ -8190,7 +8190,7 @@
         </is>
       </c>
       <c r="C518" t="n">
-        <v>3.323549337074386</v>
+        <v>4.416694834403923</v>
       </c>
     </row>
     <row r="519">
@@ -8205,7 +8205,7 @@
         </is>
       </c>
       <c r="C519" t="n">
-        <v>1.863050836187367</v>
+        <v>1.041840631636106</v>
       </c>
     </row>
     <row r="520">
@@ -8220,7 +8220,7 @@
         </is>
       </c>
       <c r="C520" t="n">
-        <v>2.529215038935226</v>
+        <v>3.664054175304699</v>
       </c>
     </row>
     <row r="521">
@@ -8235,7 +8235,7 @@
         </is>
       </c>
       <c r="C521" t="n">
-        <v>1.538160413260754</v>
+        <v>4.82586522960087</v>
       </c>
     </row>
   </sheetData>

</xml_diff>